<commit_message>
add edge cases print statements
</commit_message>
<xml_diff>
--- a/NP Data Hub Variables.xlsx
+++ b/NP Data Hub Variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rpiexchange-my.sharepoint.com/personal/ringsm_rpi_edu/Documents/Summer 2024/NP Data Hub/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mr.youssef/Desktop/NpDataHub/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="328" documentId="8_{F6944BCB-45D5-4C7A-8FC0-C948678A65BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{69804D57-6E03-4BF2-82C4-B6FFCC468C15}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF26082B-4D4B-434F-9FC2-5BA3CB8ACBEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{9E66B3E0-ECC7-4331-8FA7-D6EEB0D64780}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{9E66B3E0-ECC7-4331-8FA7-D6EEB0D64780}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="98">
   <si>
     <t>Table 1 : Non profit Organization + Private foundations Information (may separate) into 2</t>
   </si>
@@ -125,9 +125,6 @@
     <t>zipcode</t>
   </si>
   <si>
-    <t>YES</t>
-  </si>
-  <si>
     <t>Table 2 NonprofitFinancials</t>
   </si>
   <si>
@@ -141,9 +138,6 @@
   </si>
   <si>
     <t>totrevenue</t>
-  </si>
-  <si>
-    <t>revenue - expenses - assets - liabilities</t>
   </si>
   <si>
     <t>TotalAssetsEOYAmt OR TotalAssetsGrp =&gt; EOYAmt</t>
@@ -457,7 +451,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -626,14 +620,14 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -968,27 +962,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3AA55DD-E749-42C6-9E5E-99B108F9DD87}">
-  <dimension ref="A1:E61"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="128.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="63.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="59.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.1796875" style="1"/>
+    <col min="1" max="1" width="128.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="59.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1002,7 +996,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1013,7 +1007,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1027,7 +1021,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -1038,7 +1032,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -1049,7 +1043,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -1060,7 +1054,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>21</v>
       </c>
@@ -1071,18 +1065,18 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="15" t="s">
         <v>24</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
@@ -1092,318 +1086,312 @@
       <c r="C10" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="1" t="s">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A14" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="1" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A16" s="1" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="C17" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="1" t="s">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A18" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="B18" s="9" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="9" t="s">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A19" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="B19" s="8" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="8" t="s">
+    </row>
+    <row r="20" spans="1:3" ht="16" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="1" t="s">
+      <c r="C20" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="1" t="s">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A21" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="B21" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="3" t="s">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A22" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="B22" s="21" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="15" t="s">
+      <c r="C22" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="B22" s="15" t="s">
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A23" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="B23" s="22" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="15" t="s">
+      <c r="C23" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="B23" s="17" t="s">
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A24" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C23" s="15" t="s">
+      <c r="B24" s="4" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B24" s="4" t="s">
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A25" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="B25" s="4" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B25" s="4" t="s">
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A26" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="B26" s="4" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B26" s="4" t="s">
+    </row>
+    <row r="27" spans="1:3" ht="16" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="B27" s="17" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="1" t="s">
+      <c r="C27" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="B27" s="19" t="s">
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A28" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C27" s="18" t="s">
+      <c r="B28" s="17" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B28" s="19" t="s">
+    </row>
+    <row r="29" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="B29" s="18" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="1" t="s">
+      <c r="C29" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="B29" s="20" t="s">
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B30" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C29" s="21" t="s">
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A31" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="B30" s="3" t="s">
+      <c r="B31" s="7" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="1" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B32" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B31" s="7" t="s">
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B33" s="5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
-      <c r="B32" s="5" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B34" s="10" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
-      <c r="B33" s="5" t="s">
+    <row r="35" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A35" s="20" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A39" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
-      <c r="B34" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="14.5">
-      <c r="A35" s="22" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
-      <c r="A39" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B41" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B42" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B43" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B44" s="4" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
-      <c r="B43" s="6" t="s">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B45" s="4" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
-      <c r="B44" s="4" t="s">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B46" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
-      <c r="B45" s="4" t="s">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B47" s="4" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
-      <c r="B46" s="4" t="s">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B48" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
-      <c r="B47" s="4" t="s">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B49" s="4" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
-      <c r="B48" s="4" t="s">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B50" s="4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="49" spans="2:2">
-      <c r="B49" s="4" t="s">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B51" s="4" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="50" spans="2:2">
-      <c r="B50" s="4" t="s">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B52" s="4" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="51" spans="2:2">
-      <c r="B51" s="4" t="s">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B53" s="4" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="52" spans="2:2">
-      <c r="B52" s="4" t="s">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B54" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="53" spans="2:2">
-      <c r="B53" s="4" t="s">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B55" s="4" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="54" spans="2:2">
-      <c r="B54" s="1" t="s">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B56" s="4" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="55" spans="2:2">
-      <c r="B55" s="4" t="s">
+    <row r="57" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B57" s="4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="56" spans="2:2">
-      <c r="B56" s="4" t="s">
+    <row r="58" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B58" s="4" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="57" spans="2:2">
-      <c r="B57" s="4" t="s">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B59" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="58" spans="2:2">
-      <c r="B58" s="4" t="s">
+    <row r="60" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B60" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="59" spans="2:2">
-      <c r="B59" s="4" t="s">
+    <row r="61" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B61" s="1" t="s">
         <v>96</v>
-      </c>
-    </row>
-    <row r="60" spans="2:2">
-      <c r="B60" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="61" spans="2:2">
-      <c r="B61" s="1" t="s">
-        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>